<commit_message>
Felipe Neto 4_ gerado Felipe Neto 1  completo Felipe Neto2 iniciado
</commit_message>
<xml_diff>
--- a/FelipeNeto_1.xlsx
+++ b/FelipeNeto_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive - Insper - Institudo de Ensino e Pesquisa\Desktop\Insper\2°Semestre\C.Dados\Projeto_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C252C5-742A-40C2-B507-2E975429F4D5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{E0C252C5-742A-40C2-B507-2E975429F4D5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{7B648F20-AB98-4CA3-91D8-9E7D5744DF84}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1452,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="B173" sqref="B173"/>
+    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="B201" sqref="B201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2542,6 +2542,9 @@
       <c r="A136" t="s">
         <v>135</v>
       </c>
+      <c r="B136">
+        <v>4</v>
+      </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
@@ -2555,6 +2558,9 @@
       <c r="A138" t="s">
         <v>137</v>
       </c>
+      <c r="B138">
+        <v>2</v>
+      </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
@@ -2568,111 +2574,177 @@
       <c r="A140" t="s">
         <v>139</v>
       </c>
+      <c r="B140">
+        <v>3</v>
+      </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>140</v>
       </c>
+      <c r="B141">
+        <v>3</v>
+      </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>141</v>
       </c>
+      <c r="B142">
+        <v>3</v>
+      </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>142</v>
       </c>
+      <c r="B143">
+        <v>3</v>
+      </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B144">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B145">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B146">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B147">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B149">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B151">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B153">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B154">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B157">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B159">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>159</v>
+      </c>
+      <c r="B160">
+        <v>4</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>160</v>
       </c>
+      <c r="B161">
+        <v>4</v>
+      </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
@@ -2686,46 +2758,73 @@
       <c r="A163" t="s">
         <v>162</v>
       </c>
+      <c r="B163">
+        <v>3</v>
+      </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>163</v>
       </c>
+      <c r="B164">
+        <v>1</v>
+      </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>164</v>
       </c>
+      <c r="B165">
+        <v>4</v>
+      </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>165</v>
       </c>
+      <c r="B166">
+        <v>0</v>
+      </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>166</v>
       </c>
+      <c r="B167">
+        <v>3</v>
+      </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>167</v>
       </c>
+      <c r="B168">
+        <v>1</v>
+      </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>168</v>
       </c>
+      <c r="B169">
+        <v>3</v>
+      </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>169</v>
       </c>
+      <c r="B170">
+        <v>1</v>
+      </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>170</v>
       </c>
+      <c r="B171">
+        <v>1</v>
+      </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
@@ -2739,11 +2838,17 @@
       <c r="A173" t="s">
         <v>172</v>
       </c>
+      <c r="B173">
+        <v>3</v>
+      </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>173</v>
       </c>
+      <c r="B174">
+        <v>0</v>
+      </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
@@ -2773,21 +2878,33 @@
       <c r="A178" t="s">
         <v>177</v>
       </c>
+      <c r="B178">
+        <v>0</v>
+      </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>178</v>
       </c>
+      <c r="B179">
+        <v>3</v>
+      </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>179</v>
       </c>
+      <c r="B180">
+        <v>1</v>
+      </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>180</v>
       </c>
+      <c r="B181">
+        <v>3</v>
+      </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
@@ -2801,66 +2918,105 @@
       <c r="A183" t="s">
         <v>182</v>
       </c>
+      <c r="B183">
+        <v>2</v>
+      </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>183</v>
       </c>
+      <c r="B184">
+        <v>1</v>
+      </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>184</v>
       </c>
+      <c r="B185">
+        <v>2</v>
+      </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>185</v>
       </c>
+      <c r="B186">
+        <v>3</v>
+      </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>186</v>
       </c>
+      <c r="B187">
+        <v>4</v>
+      </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>187</v>
       </c>
+      <c r="B188">
+        <v>3</v>
+      </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>188</v>
       </c>
+      <c r="B189">
+        <v>2</v>
+      </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>189</v>
       </c>
+      <c r="B190">
+        <v>1</v>
+      </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>190</v>
       </c>
+      <c r="B191">
+        <v>2</v>
+      </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>191</v>
       </c>
+      <c r="B192">
+        <v>2</v>
+      </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>192</v>
       </c>
+      <c r="B193">
+        <v>1</v>
+      </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>193</v>
       </c>
+      <c r="B194">
+        <v>2</v>
+      </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>194</v>
       </c>
+      <c r="B195">
+        <v>3</v>
+      </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
@@ -2874,20 +3030,32 @@
       <c r="A197" t="s">
         <v>196</v>
       </c>
+      <c r="B197">
+        <v>3</v>
+      </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>197</v>
       </c>
+      <c r="B198">
+        <v>4</v>
+      </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>198</v>
       </c>
+      <c r="B199">
+        <v>4</v>
+      </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>199</v>
+      </c>
+      <c r="B200">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>